<commit_message>
Changes to be committed: 	modified:   Create Graphs 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2020 Datasheets & Spreadsheets_combined.xlsx 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2022 Datasheets & Spreadsheets_combined.xlsx 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2023 Datasheets & Spreadsheets_combined.xlsx 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2024 Datasheets & Spreadsheets_combined.xlsx
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform - Color-wise graphs/2020 Datasheets & Spreadsheets_combined.xlsx
+++ b/Extracted Data/VRU Headform - Color-wise graphs/2020 Datasheets & Spreadsheets_combined.xlsx
@@ -24,13 +24,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -41,7 +44,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -49,12 +52,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -420,14 +432,27 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Input Sheet</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -438,14 +463,27 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Input Sheet</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -456,14 +494,27 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Input Sheet</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -474,14 +525,27 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Input Sheet</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -492,14 +556,27 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Input Sheet</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -510,14 +587,27 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Input Sheet</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -528,14 +618,27 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Input Sheet</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -546,14 +649,27 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Input Sheet</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes to be committed: 	modified:   Create Graphs 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2020 Datasheets & Spreadsheets_combined.xlsx 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2023 Datasheets & Spreadsheets_combined.xlsx 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2024 Datasheets & Spreadsheets_combined.xlsx
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform - Color-wise graphs/2020 Datasheets & Spreadsheets_combined.xlsx
+++ b/Extracted Data/VRU Headform - Color-wise graphs/2020 Datasheets & Spreadsheets_combined.xlsx
@@ -443,12 +443,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Input Sheet</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>
@@ -474,12 +474,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Input Sheet</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>
@@ -505,12 +505,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Input Sheet</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>
@@ -536,12 +536,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Input Sheet</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>
@@ -567,12 +567,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Input Sheet</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>
@@ -598,12 +598,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Input Sheet</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>
@@ -629,12 +629,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Input Sheet</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>
@@ -660,12 +660,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Input Sheet</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
modified:   Create Graphs 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2020 Datasheets & Spreadsheets_combined.xlsx
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform - Color-wise graphs/2020 Datasheets & Spreadsheets_combined.xlsx
+++ b/Extracted Data/VRU Headform - Color-wise graphs/2020 Datasheets & Spreadsheets_combined.xlsx
@@ -1,39 +1,14 @@
-
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
-  <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Default green" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Green" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Yellow" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Orange" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Brown" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Red" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Default Red" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Blue" sheetId="8" state="visible" r:id="rId8"/>
-  </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
-</workbook>
-</file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -44,7 +19,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -52,21 +27,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -424,252 +390,4 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
-</file>
-
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Car Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Values</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Car Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Values</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Car Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Values</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Car Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Values</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Car Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Values</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Car Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Values</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Car Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Values</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Car Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Values</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes to be committed: 	deleted:    Create Graphs 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2020 Datasheets & Spreadsheets_combined.xlsx 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2022 Datasheets & Spreadsheets_combined.xlsx 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2023 Datasheets & Spreadsheets_combined.xlsx 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2024 Datasheets & Spreadsheets_combined.xlsx 	new file:   Output file with Sheet names
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform - Color-wise graphs/2020 Datasheets & Spreadsheets_combined.xlsx
+++ b/Extracted Data/VRU Headform - Color-wise graphs/2020 Datasheets & Spreadsheets_combined.xlsx
@@ -1,3 +1,25 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Default green" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Green" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Yellow" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Orange" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Brown" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Red" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Default Red" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Blue" sheetId="8" state="visible" r:id="rId8"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
+</file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
@@ -390,4 +412,148 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes to be committed: 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2020 Datasheets & Spreadsheets_combined.xlsx 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2022 Datasheets & Spreadsheets_combined.xlsx 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2023 Datasheets & Spreadsheets_combined.xlsx 	modified:   Extracted Data/VRU Headform - Color-wise graphs/2024 Datasheets & Spreadsheets_combined.xlsx 	modified:   Output file with Sheet names
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform - Color-wise graphs/2020 Datasheets & Spreadsheets_combined.xlsx
+++ b/Extracted Data/VRU Headform - Color-wise graphs/2020 Datasheets & Spreadsheets_combined.xlsx
@@ -420,14 +420,107 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Toyota Yaris</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Mazda MX-30</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Honda JAZZ</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Land Rover Defender</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SEAT Leon</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>KIA Sorento</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Honda e</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Hyundai i10</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ISUZU D-Max Crew Cab</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Audi A3</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -438,14 +531,107 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Toyota Yaris</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Mazda MX-30</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Honda JAZZ</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Land Rover Defender</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SEAT Leon</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>KIA Sorento</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Honda e</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Hyundai i10</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ISUZU D-Max Crew Cab</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Audi A3</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -456,14 +642,107 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Toyota Yaris</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Mazda MX-30</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Honda JAZZ</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Land Rover Defender</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SEAT Leon</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>KIA Sorento</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Honda e</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Hyundai i10</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ISUZU D-Max Crew Cab</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Audi A3</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -474,14 +753,107 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Toyota Yaris</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Mazda MX-30</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Honda JAZZ</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Land Rover Defender</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SEAT Leon</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>KIA Sorento</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Honda e</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Hyundai i10</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ISUZU D-Max Crew Cab</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Audi A3</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -492,14 +864,107 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Toyota Yaris</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Mazda MX-30</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Honda JAZZ</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Land Rover Defender</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SEAT Leon</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>KIA Sorento</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Honda e</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Hyundai i10</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ISUZU D-Max Crew Cab</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Audi A3</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -510,14 +975,107 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Toyota Yaris</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Mazda MX-30</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Honda JAZZ</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Land Rover Defender</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SEAT Leon</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>KIA Sorento</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Honda e</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Hyundai i10</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ISUZU D-Max Crew Cab</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Audi A3</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -528,14 +1086,107 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Toyota Yaris</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Mazda MX-30</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Honda JAZZ</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Land Rover Defender</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SEAT Leon</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>KIA Sorento</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Honda e</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Hyundai i10</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ISUZU D-Max Crew Cab</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Audi A3</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -546,14 +1197,107 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Car Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Toyota Yaris</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Mazda MX-30</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Honda JAZZ</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Land Rover Defender</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SEAT Leon</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>KIA Sorento</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Honda e</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Hyundai i10</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ISUZU D-Max Crew Cab</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Audi A3</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>